<commit_message>
Finished module 2 Takeoffs and Landings and am uploading the notes
</commit_message>
<xml_diff>
--- a/Sportys/Video Record.xlsx
+++ b/Sportys/Video Record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Documents\Pilot-Training\Sportys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E16A48-7F4B-406A-8021-BE9C04964C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E2EAB8-740A-45C8-94BF-D206B9E364C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -118,6 +118,45 @@
   </si>
   <si>
     <t>Practicing Landings</t>
+  </si>
+  <si>
+    <t>Ground Reference Manuevers</t>
+  </si>
+  <si>
+    <t>Closer Look: Taxi Tips</t>
+  </si>
+  <si>
+    <t>Engines</t>
+  </si>
+  <si>
+    <t>Air Facts: Engine Suspicion</t>
+  </si>
+  <si>
+    <t>Aerodynamics</t>
+  </si>
+  <si>
+    <t>Air Closer Look: Angle of Attack</t>
+  </si>
+  <si>
+    <t>Slow Flight</t>
+  </si>
+  <si>
+    <t>Closer Look: Change of Scenery</t>
+  </si>
+  <si>
+    <t>Stalls</t>
+  </si>
+  <si>
+    <t>Air Facts:Stall Rhetoric</t>
+  </si>
+  <si>
+    <t>2/21/20223</t>
+  </si>
+  <si>
+    <t>Normal Landings</t>
+  </si>
+  <si>
+    <t>Air Facts: Down to Earth</t>
   </si>
 </sst>
 </file>
@@ -457,16 +496,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.81640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -770,10 +809,134 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>44874</v>
+        <v>44876</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>44876</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>44876</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>44876</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>44878</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>44878</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>44878</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>44878</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>44976</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>44978</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Your first solo lesson 17: Thunderstorms complete
</commit_message>
<xml_diff>
--- a/Sportys/Video Record.xlsx
+++ b/Sportys/Video Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Pilot-Training\Sportys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A286A4CC-9A06-4096-93CB-8D6D700684D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED36A170-B2A5-4918-BDFD-54FE4722DC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t>Terminal Aerodrome Forecast (TAF)</t>
+  </si>
+  <si>
+    <t>Closer Look: Get the Big Picture</t>
+  </si>
+  <si>
+    <t>Intro to Glass Cockpit Systems</t>
+  </si>
+  <si>
+    <t>Airport Signs and Markings</t>
   </si>
 </sst>
 </file>
@@ -532,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+      <selection pane="bottomLeft" activeCell="J38" sqref="J38:J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,6 +1105,39 @@
         <v>55</v>
       </c>
     </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>45042</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>45042</v>
+      </c>
+      <c r="B52" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B53" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Your First Solo Lesson 18: Radar Imagery completed
</commit_message>
<xml_diff>
--- a/Sportys/Video Record.xlsx
+++ b/Sportys/Video Record.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Pilot-Training\Sportys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED36A170-B2A5-4918-BDFD-54FE4722DC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18316D9E-C8CA-4941-83E0-DF28ECEC455D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>Airport Signs and Markings</t>
+  </si>
+  <si>
+    <t>Radar Imagery</t>
+  </si>
+  <si>
+    <t>Thunderstorms and Convective Forecasts</t>
   </si>
 </sst>
 </file>
@@ -541,18 +547,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J38" sqref="J38:J40"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1138,6 +1144,28 @@
         <v>58</v>
       </c>
     </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>45049</v>
+      </c>
+      <c r="B54" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>45050</v>
+      </c>
+      <c r="B55" t="s">
+        <v>49</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed lessons up to 21 Thrust, Weight, and Stability
</commit_message>
<xml_diff>
--- a/Sportys/Video Record.xlsx
+++ b/Sportys/Video Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Pilot-Training\Sportys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18316D9E-C8CA-4941-83E0-DF28ECEC455D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FFA1E1-1AC8-4EAE-BCD5-24AD98D7E355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>Thunderstorms and Convective Forecasts</t>
+  </si>
+  <si>
+    <t>Drag</t>
+  </si>
+  <si>
+    <t>A closer look : Reducing Drag</t>
+  </si>
+  <si>
+    <t>Thrust,Stability, and Center of Gravity</t>
+  </si>
+  <si>
+    <t>Flight service Weather Briefings</t>
   </si>
 </sst>
 </file>
@@ -547,11 +559,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
+      <selection pane="bottomLeft" activeCell="Q43" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,6 +1178,50 @@
         <v>59</v>
       </c>
     </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B58" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B59" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
completed my first solo
</commit_message>
<xml_diff>
--- a/Sportys/Video Record.xlsx
+++ b/Sportys/Video Record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Pilot-Training\Sportys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FFA1E1-1AC8-4EAE-BCD5-24AD98D7E355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF90A061-2E30-4AC4-93E2-BEEBEAE1C523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -220,6 +220,21 @@
   </si>
   <si>
     <t>Flight service Weather Briefings</t>
+  </si>
+  <si>
+    <t>Collision Avoidance</t>
+  </si>
+  <si>
+    <t>Student Pilot &amp; Medical Cetificate</t>
+  </si>
+  <si>
+    <t>Air Facts: Fit for Flight</t>
+  </si>
+  <si>
+    <t>Solo</t>
+  </si>
+  <si>
+    <t>Your Dual Cross Countries</t>
   </si>
 </sst>
 </file>
@@ -559,17 +574,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q43" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1222,6 +1237,58 @@
         <v>64</v>
       </c>
     </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>45052</v>
+      </c>
+      <c r="B60" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>45168</v>
+      </c>
+      <c r="B61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>45168</v>
+      </c>
+      <c r="B62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>45168</v>
+      </c>
+      <c r="B63" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>45169</v>
+      </c>
+      <c r="B64" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>